<commit_message>
chore: updates dependencies @commitlint/cli                            ~17.4.2  →  ~19.8.1 @commitlint/config-conventional            ~17.4.2  →  ~19.8.1 @semantic-release/changelog                 ~6.0.2  →   ~6.0.3 @semantic-release/commit-analyzer           ~9.0.2  →  ~13.0.1 @semantic-release/exec                      ~6.0.3  →   ~7.1.0 @semantic-release/github                    ~8.0.7  →  ~11.0.3 @semantic-release/npm                       ~9.0.2  →  ~12.0.1 @semantic-release/release-notes-generator  ~10.0.3  →  ~14.0.3 ava                                         ~5.1.1  →   ~6.3.0 c8                                         ~7.12.0  →  ~10.1.3 commitizen                                  ~4.3.0  →   ~4.3.1 eslint                                     ~8.33.0  →  ~9.27.0 husky                                       ~8.0.3  →   ~9.1.7
</commit_message>
<xml_diff>
--- a/test/data/normal-test-input.xlsx
+++ b/test/data/normal-test-input.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Header 1</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>Gifs make me smile</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>Baz</t>
   </si>
 </sst>
 </file>
@@ -117,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -317,13 +329,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -385,6 +434,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -636,7 +694,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -666,7 +723,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -692,7 +748,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -718,7 +773,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -744,7 +798,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -770,7 +823,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -796,7 +848,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -822,7 +873,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -848,7 +898,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -874,7 +923,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -925,7 +973,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -951,7 +998,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -977,7 +1023,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1003,7 +1048,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1029,7 +1073,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1055,7 +1098,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1081,7 +1123,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1107,7 +1148,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1133,7 +1173,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1159,7 +1198,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1207,7 +1245,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1237,7 +1274,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1263,7 +1299,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1289,7 +1324,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1315,7 +1349,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1341,7 +1374,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1367,7 +1399,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1393,7 +1424,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1419,7 +1449,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1445,7 +1474,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1474,7 +1502,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1551,18 +1579,28 @@
       </c>
     </row>
     <row r="5" ht="14.7" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s" s="8">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" ht="14.7" customHeight="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" ht="14.7" customHeight="1">
       <c r="A7" s="15"/>
@@ -1579,11 +1617,25 @@
       <c r="E8" s="17"/>
     </row>
     <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="20"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" ht="14.7" customHeight="1">
+      <c r="A11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>